<commit_message>
Addressed feedback elements accordingly (except two -> need feedback for that)
</commit_message>
<xml_diff>
--- a/feedback.xlsx
+++ b/feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Holthausen Solutions\onepager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBC7A153-E2C1-4453-AEC7-C5E42399A8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9615E18A-DE38-4377-8D84-7CAF86F97ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7682148E-B450-444B-9048-4162FC3CA47C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7682148E-B450-444B-9048-4162FC3CA47C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>anchor link nicht mit offset</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>background on carousel wrong way?</t>
+  </si>
+  <si>
+    <t>Rücksprache</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="A2:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +463,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -468,6 +472,7 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -476,6 +481,9 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -493,6 +501,9 @@
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -501,6 +512,7 @@
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -509,6 +521,7 @@
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -517,6 +530,7 @@
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -525,6 +539,7 @@
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -551,6 +566,7 @@
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -559,6 +575,7 @@
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -567,6 +584,7 @@
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -575,6 +593,7 @@
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -583,6 +602,7 @@
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>